<commit_message>
Report(Actual Order Amount & Order Balance) updated: add the content
</commit_message>
<xml_diff>
--- a/XLSX/ActualOrderAmountOrderBalance.xlsx
+++ b/XLSX/ActualOrderAmountOrderBalance.xlsx
@@ -1,52 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <x:workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\Hagiwara\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C98574-2874-4E25-9473-C960A905157F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="SalesLine1" sheetId="5" r:id="rId1"/>
-    <x:sheet name="SalesLine2" sheetId="6" r:id="rId2"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension Id from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ObjectCaption" comment="Use this function to get the Object Caption from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Caption",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company Display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.DateLocal" comment="Use this function to get the Date (Local) from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date (Local)",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",#REF!,#REF!,"none")</x:definedName>
-    <x:definedName name="ReportRequest.UTCOffset" comment="Use this function to get the UTC Offset from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("UTC Offset",#REF!,#REF!,"none")</x:definedName>
-  </x:definedNames>
-  <x:calcPr calcId="191029"/>
-  <x:extLst>
-    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2090061-9E39-4B81-9A46-32AC9609E983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="DateSheet" sheetId="5" r:id="rId1"/>
+    <sheet name="RemainingSalesOrder" sheetId="6" r:id="rId2"/>
+    <sheet name="SalesOrderActual" sheetId="7" r:id="rId3"/>
+    <sheet name="SalesOrderBalanceSheet" sheetId="8" r:id="rId4"/>
+    <sheet name="CustomerSheet" sheetId="9" r:id="rId5"/>
+  </sheets>
+  <definedNames>
+    <definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension Id from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ObjectCaption" comment="Use this function to get the Object Caption from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Caption",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company Display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.DateLocal" comment="Use this function to get the Date (Local) from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date (Local)",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",#REF!,#REF!,"none")</definedName>
+    <definedName name="ReportRequest.UTCOffset" comment="Use this function to get the UTC Offset from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("UTC Offset",#REF!,#REF!,"none")</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -56,13 +59,19 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+  <si>
+    <t>StartDate</t>
+  </si>
+  <si>
+    <t>EndDate</t>
+  </si>
   <si>
     <t>DocumentType</t>
   </si>
@@ -73,22 +82,262 @@
     <t>SelltoCustomerNo</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>CustomerItemNo</t>
+  </si>
+  <si>
+    <t>PartsNo</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>OEMNo</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>PromisedDeliveryDate1</t>
+  </si>
+  <si>
+    <t>RequestedDeliveryDate1</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>CustomerOrderNo</t>
+  </si>
+  <si>
+    <t>LocationCode</t>
+  </si>
+  <si>
+    <t>Reserve</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>ReservedQtyBase</t>
+  </si>
+  <si>
+    <t>FullyReserved</t>
+  </si>
+  <si>
+    <t>UnitofMeasureCode</t>
+  </si>
+  <si>
+    <t>UnitPriceExcl_VAT</t>
+  </si>
+  <si>
+    <t>UnitCost</t>
+  </si>
+  <si>
+    <t>UnitCost_LCY</t>
+  </si>
+  <si>
+    <t>LineAmountExclVAT</t>
+  </si>
+  <si>
+    <t>LineAmountExclVATLCY</t>
+  </si>
+  <si>
+    <t>ShipmentDate</t>
+  </si>
+  <si>
+    <t>OutstandingQuantity</t>
+  </si>
+  <si>
+    <t>OutstandingQtyBase</t>
+  </si>
+  <si>
+    <t>Calculated</t>
+  </si>
+  <si>
+    <t>CustomerPostingGroup</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>CustomerItemNo</t>
-  </si>
-  <si>
-    <t>PartsNo</t>
-  </si>
-  <si>
-    <t>Rank</t>
+    <t>False</t>
+  </si>
+  <si>
+    <t>ShipmentDate111</t>
+  </si>
+  <si>
+    <t>PostingDate</t>
+  </si>
+  <si>
+    <t>DocumentDate</t>
+  </si>
+  <si>
+    <t>No111</t>
+  </si>
+  <si>
+    <t>CustomerNo</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>OrderNo</t>
+  </si>
+  <si>
+    <t>OEMNo111</t>
+  </si>
+  <si>
+    <t>OEMName</t>
+  </si>
+  <si>
+    <t>CurrencyCode</t>
+  </si>
+  <si>
+    <t>DueDate</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>AmountLCY</t>
+  </si>
+  <si>
+    <t>AmountIncludingVAT</t>
+  </si>
+  <si>
+    <t>ExternalDocumentNo</t>
+  </si>
+  <si>
+    <t>RemainingAmount</t>
+  </si>
+  <si>
+    <t>LocationCode111</t>
+  </si>
+  <si>
+    <t>PrintedNo</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Cancelled</t>
+  </si>
+  <si>
+    <t>Corrective</t>
+  </si>
+  <si>
+    <t>ShipmentMethodCode</t>
+  </si>
+  <si>
+    <t>CustomerGroupCode</t>
+  </si>
+  <si>
+    <t>CustomerPostingGroup111</t>
+  </si>
+  <si>
+    <t>ShipmentDate222222</t>
+  </si>
+  <si>
+    <t>PostingDate222</t>
+  </si>
+  <si>
+    <t>DocumentDate222</t>
+  </si>
+  <si>
+    <t>No222</t>
+  </si>
+  <si>
+    <t>CustomerNo222</t>
+  </si>
+  <si>
+    <t>Customer222</t>
+  </si>
+  <si>
+    <t>OrderNo222</t>
+  </si>
+  <si>
+    <t>OEMNo222</t>
+  </si>
+  <si>
+    <t>OEMName222</t>
+  </si>
+  <si>
+    <t>CurrencyCode222</t>
+  </si>
+  <si>
+    <t>DueDate222</t>
+  </si>
+  <si>
+    <t>Amount222</t>
+  </si>
+  <si>
+    <t>AmountLCY222</t>
+  </si>
+  <si>
+    <t>AmountIncludingVAT222</t>
+  </si>
+  <si>
+    <t>ExternalDocumentNo222</t>
+  </si>
+  <si>
+    <t>RemainingAmount222</t>
+  </si>
+  <si>
+    <t>LocationCode222</t>
+  </si>
+  <si>
+    <t>PrintedNo222</t>
+  </si>
+  <si>
+    <t>Closed222</t>
+  </si>
+  <si>
+    <t>Cancelled222</t>
+  </si>
+  <si>
+    <t>Corrective222</t>
+  </si>
+  <si>
+    <t>ShipmentMethodCode222</t>
+  </si>
+  <si>
+    <t>CustomerGroupCode222</t>
+  </si>
+  <si>
+    <t>CustomerPostingGroup222</t>
+  </si>
+  <si>
+    <t>No333</t>
+  </si>
+  <si>
+    <t>FamiliarName</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>CountryRegionCode</t>
+  </si>
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>CustomerPostingGroup333</t>
+  </si>
+  <si>
+    <t>ShipmentMethodCode333</t>
+  </si>
+  <si>
+    <t>ShippingAgentCode</t>
   </si>
 </sst>
 </file>
@@ -123,13 +372,91 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC0C0C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC0C0C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFC0C0C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -194,29 +521,137 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="SalesLine1" displayName="SalesLine1" ref="A1:C2" totalsRowShown="0" headerRowDxfId="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:C2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="3">
-    <x:tableColumn id="1" name="DocumentType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="DocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="3" name="SelltoCustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="DateSheet" displayName="DateSheet" ref="A1:B2" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:B2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="StartDate"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EndDate"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="SalesLine2" displayName="SalesLine2" ref="A1:E2" totalsRowShown="0" headerRowDxfId="0" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:E2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="5">
-    <x:tableColumn id="1" name="Type" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="3" name="CustomerItemNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="4" name="PartsNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="5" name="Rank" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentType"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentNo"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SelltoCustomerNo"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Type"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerItemNo"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PartsNo"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Rank"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Products"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMNo"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrderDate"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PromisedDeliveryDate1"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RequestedDeliveryDate1"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Description"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerOrderNo"/>
+    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LocationCode"/>
+    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Reserve"/>
+    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity"/>
+    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReservedQtyBase"/>
+    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="FullyReserved"/>
+    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitofMeasureCode"/>
+    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitPriceExcl_VAT"/>
+    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitCost"/>
+    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitCost_LCY"/>
+    <tableColumn id="25" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LineAmountExclVAT"/>
+    <tableColumn id="26" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LineAmountExclVATLCY"/>
+    <tableColumn id="27" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentDate"/>
+    <tableColumn id="28" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OutstandingQuantity"/>
+    <tableColumn id="29" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OutstandingQtyBase"/>
+    <tableColumn id="30" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Calculated"/>
+    <tableColumn id="31" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentDate111"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PostingDate"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentDate"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No111"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerNo"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Customer"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrderNo"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMNo111"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMName"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CurrencyCode"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DueDate"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Amount"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountLCY"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountIncludingVAT"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ExternalDocumentNo"/>
+    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingAmount"/>
+    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LocationCode111"/>
+    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PrintedNo"/>
+    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Closed"/>
+    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Cancelled"/>
+    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Corrective"/>
+    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentMethodCode"/>
+    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerGroupCode"/>
+    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup111"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="SalesOrderBalanceSheet" displayName="SalesOrderBalanceSheet" ref="A1:X2" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentDate222222"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PostingDate222"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentDate222"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No222"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerNo222"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Customer222"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrderNo222"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMNo222"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMName222"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CurrencyCode222"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DueDate222"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Amount222"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountLCY222"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountIncludingVAT222"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ExternalDocumentNo222"/>
+    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingAmount222"/>
+    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LocationCode222"/>
+    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PrintedNo222"/>
+    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Closed222"/>
+    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Cancelled222"/>
+    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Corrective222"/>
+    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentMethodCode222"/>
+    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerGroupCode222"/>
+    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup222"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No333"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="FamiliarName"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Name"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CountryRegionCode"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="County"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup333"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentMethodCode333"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShippingAgentCode"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -515,11 +950,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C906EA-A277-4986-A47F-BC66D34064DD}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD324A-2965-41B1-8AFF-2478309124C6}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -527,26 +962,20 @@
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -558,8 +987,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA45ADC1-CDFE-428A-83E9-BDA6A2C713B8}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56161066-9B38-4DD3-A0DA-EC70538AD125}">
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -568,38 +997,599 @@
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>18</v>
+      </c>
+      <c r="R1" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
+        <v>23</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF22EC56-EE68-4288-9303-7A32AEBCCC8E}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
+        <v>52</v>
+      </c>
+      <c r="S1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" t="s">
+        <v>56</v>
+      </c>
+      <c r="W1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X1" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AC93CF-A70D-4E86-AA46-4AE1A32EDE8E}">
+  <dimension ref="A1:X2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>75</v>
+      </c>
+      <c r="R1" t="s">
+        <v>76</v>
+      </c>
+      <c r="S1" t="s">
+        <v>77</v>
+      </c>
+      <c r="T1" t="s">
+        <v>78</v>
+      </c>
+      <c r="U1" t="s">
+        <v>79</v>
+      </c>
+      <c r="V1" t="s">
+        <v>80</v>
+      </c>
+      <c r="W1" t="s">
+        <v>81</v>
+      </c>
+      <c r="X1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCE851F-52AC-4D40-872D-5DA20E49CF56}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Report(Actual Order Amount & Order Balance) updated: add the filter etc.
</commit_message>
<xml_diff>
--- a/XLSX/ActualOrderAmountOrderBalance.xlsx
+++ b/XLSX/ActualOrderAmountOrderBalance.xlsx
@@ -1,55 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <x:workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\Hagiwara\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2090061-9E39-4B81-9A46-32AC9609E983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="DateSheet" sheetId="5" r:id="rId1"/>
-    <sheet name="RemainingSalesOrder" sheetId="6" r:id="rId2"/>
-    <sheet name="SalesOrderActual" sheetId="7" r:id="rId3"/>
-    <sheet name="SalesOrderBalanceSheet" sheetId="8" r:id="rId4"/>
-    <sheet name="CustomerSheet" sheetId="9" r:id="rId5"/>
-  </sheets>
-  <definedNames>
-    <definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension Id from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ObjectCaption" comment="Use this function to get the Object Caption from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Caption",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company Display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.DateLocal" comment="Use this function to get the Date (Local) from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date (Local)",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",#REF!,#REF!,"none")</definedName>
-    <definedName name="ReportRequest.UTCOffset" comment="Use this function to get the UTC Offset from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("UTC Offset",#REF!,#REF!,"none")</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CA7CE6-D2C4-46E7-AD06-93EAF2AFA7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="DateSheet" sheetId="5" r:id="rId1"/>
+    <x:sheet name="RemainingSalesOrder" sheetId="6" state="hidden" r:id="rId2"/>
+    <x:sheet name="RemainingSalesOrderPresent" sheetId="10" r:id="rId3"/>
+    <x:sheet name="SalesOrderActual" sheetId="7" r:id="rId4"/>
+    <x:sheet name="SalesOrderBalanceSheet" sheetId="8" r:id="rId5"/>
+    <x:sheet name="CustomerSheet" sheetId="9" r:id="rId6"/>
+  </x:sheets>
+  <x:definedNames>
+    <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension Id from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectCaption" comment="Use this function to get the Object Caption from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Caption",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company Display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.DateLocal" comment="Use this function to get the Date (Local) from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date (Local)",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",#REF!,#REF!,"none")</x:definedName>
+    <x:definedName name="ReportRequest.UTCOffset" comment="Use this function to get the UTC Offset from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("UTC Offset",#REF!,#REF!,"none")</x:definedName>
+  </x:definedNames>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -59,13 +60,35 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
   <si>
     <t>StartDate</t>
   </si>
@@ -338,6 +361,12 @@
   </si>
   <si>
     <t>ShippingAgentCode</t>
+  </si>
+  <si>
+    <t>Document Type</t>
+  </si>
+  <si>
+    <t>Document No.</t>
   </si>
 </sst>
 </file>
@@ -521,137 +550,137 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="DateSheet" displayName="DateSheet" ref="A1:B2" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:B2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="StartDate"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EndDate"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="DateSheet" displayName="DateSheet" ref="A1:B2" totalsRowShown="0" headerRowDxfId="4" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:B2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="2">
+    <x:tableColumn id="1" name="StartDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="EndDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="3">
-  <autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="31">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentType"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentNo"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SelltoCustomerNo"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Type"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerItemNo"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PartsNo"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Rank"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Products"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMNo"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrderDate"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PromisedDeliveryDate1"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RequestedDeliveryDate1"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Description"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerOrderNo"/>
-    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LocationCode"/>
-    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Reserve"/>
-    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Quantity"/>
-    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReservedQtyBase"/>
-    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="FullyReserved"/>
-    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitofMeasureCode"/>
-    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitPriceExcl_VAT"/>
-    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitCost"/>
-    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="UnitCost_LCY"/>
-    <tableColumn id="25" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LineAmountExclVAT"/>
-    <tableColumn id="26" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LineAmountExclVATLCY"/>
-    <tableColumn id="27" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentDate"/>
-    <tableColumn id="28" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OutstandingQuantity"/>
-    <tableColumn id="29" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OutstandingQtyBase"/>
-    <tableColumn id="30" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Calculated"/>
-    <tableColumn id="31" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="3" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="31">
+    <x:tableColumn id="1" name="DocumentType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="DocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="SelltoCustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="Type" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="CustomerItemNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="PartsNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="Rank" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="9" name="Products" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="10" name="OEMNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="11" name="OrderDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="12" name="PromisedDeliveryDate1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="13" name="RequestedDeliveryDate1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="14" name="Description" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="15" name="CustomerOrderNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="16" name="LocationCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="17" name="Reserve" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="18" name="Quantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="19" name="ReservedQtyBase" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="20" name="FullyReserved" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="21" name="UnitofMeasureCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="22" name="UnitPriceExcl_VAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="23" name="UnitCost" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="24" name="UnitCost_LCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="25" name="LineAmountExclVAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="26" name="LineAmountExclVATLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="27" name="ShipmentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="28" name="OutstandingQuantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="29" name="OutstandingQtyBase" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="30" name="Calculated" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="31" name="CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentDate111"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PostingDate"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentDate"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No111"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerNo"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Customer"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrderNo"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMNo111"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMName"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CurrencyCode"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DueDate"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Amount"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountLCY"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountIncludingVAT"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ExternalDocumentNo"/>
-    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingAmount"/>
-    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LocationCode111"/>
-    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PrintedNo"/>
-    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Closed"/>
-    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Cancelled"/>
-    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Corrective"/>
-    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentMethodCode"/>
-    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerGroupCode"/>
-    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup111"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="24">
+    <x:tableColumn id="1" name="ShipmentDate111" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="PostingDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="DocumentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="No111" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="CustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="Customer" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="OrderNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="OEMNo111" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="9" name="OEMName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="10" name="CurrencyCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="11" name="DueDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="12" name="Amount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="13" name="AmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="14" name="AmountIncludingVAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="15" name="ExternalDocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="16" name="RemainingAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="17" name="LocationCode111" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="18" name="PrintedNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="19" name="Closed" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="20" name="Cancelled" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="21" name="Corrective" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="22" name="ShipmentMethodCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="23" name="CustomerGroupCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="24" name="CustomerPostingGroup111" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="SalesOrderBalanceSheet" displayName="SalesOrderBalanceSheet" ref="A1:X2" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentDate222222"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PostingDate222"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DocumentDate222"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No222"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerNo222"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Customer222"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OrderNo222"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMNo222"/>
-    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="OEMName222"/>
-    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CurrencyCode222"/>
-    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="DueDate222"/>
-    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Amount222"/>
-    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountLCY222"/>
-    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AmountIncludingVAT222"/>
-    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ExternalDocumentNo222"/>
-    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="RemainingAmount222"/>
-    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="LocationCode222"/>
-    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="PrintedNo222"/>
-    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Closed222"/>
-    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Cancelled222"/>
-    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Corrective222"/>
-    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentMethodCode222"/>
-    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerGroupCode222"/>
-    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup222"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SalesOrderBalanceSheet" displayName="SalesOrderBalanceSheet" ref="A1:X2" totalsRowShown="0" headerRowDxfId="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="24">
+    <x:tableColumn id="1" name="ShipmentDate222222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="PostingDate222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="DocumentDate222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="No222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="CustomerNo222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="Customer222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="OrderNo222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="OEMNo222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="9" name="OEMName222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="10" name="CurrencyCode222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="11" name="DueDate222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="12" name="Amount222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="13" name="AmountLCY222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="14" name="AmountIncludingVAT222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="15" name="ExternalDocumentNo222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="16" name="RemainingAmount222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="17" name="LocationCode222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="18" name="PrintedNo222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="19" name="Closed222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="20" name="Cancelled222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="21" name="Corrective222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="22" name="ShipmentMethodCode222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="23" name="CustomerGroupCode222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="24" name="CustomerPostingGroup222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:H2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No333"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="FamiliarName"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="Name"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CountryRegionCode"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="County"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CustomerPostingGroup333"/>
-    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShipmentMethodCode333"/>
-    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ShippingAgentCode"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:H2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="8">
+    <x:tableColumn id="1" name="No333" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="2" name="FamiliarName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="3" name="Name" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="4" name="CountryRegionCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="5" name="County" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="6" name="CustomerPostingGroup333" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="7" name="ShipmentMethodCode333" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="8" name="ShippingAgentCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+  </x:tableColumns>
+  <x:tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -953,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD324A-2965-41B1-8AFF-2478309124C6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -990,7 +1019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56161066-9B38-4DD3-A0DA-EC70538AD125}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1196,10 +1227,134 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805EF4CF-BE6F-49F8-8F1B-CC10C3643A3F}">
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:AE2">RemainingSalesOrder[]</f>
+        <v/>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v/>
+      </c>
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <v/>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="str">
+        <v>False</v>
+      </c>
+      <c r="U2" t="str">
+        <v/>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF22EC56-EE68-4288-9303-7A32AEBCCC8E}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1362,7 +1517,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AC93CF-A70D-4E86-AA46-4AE1A32EDE8E}">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -1529,11 +1684,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCE851F-52AC-4D40-872D-5DA20E49CF56}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
Report(Actual Order Amount & Order Balance) updated: request page and and function for Line Amount Excl. VAT (LCY)
</commit_message>
<xml_diff>
--- a/XLSX/ActualOrderAmountOrderBalance.xlsx
+++ b/XLSX/ActualOrderAmountOrderBalance.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\Hagiwara\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40CA7CE6-D2C4-46E7-AD06-93EAF2AFA7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F09D68E1-D1A3-42E4-893B-03F4586ED083}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="DateSheet" sheetId="5" r:id="rId1"/>
-    <x:sheet name="RemainingSalesOrder" sheetId="6" state="hidden" r:id="rId2"/>
-    <x:sheet name="RemainingSalesOrderPresent" sheetId="10" r:id="rId3"/>
-    <x:sheet name="SalesOrderActual" sheetId="7" r:id="rId4"/>
-    <x:sheet name="SalesOrderBalanceSheet" sheetId="8" r:id="rId5"/>
-    <x:sheet name="CustomerSheet" sheetId="9" r:id="rId6"/>
+    <x:sheet name="RemainingSalesOrder" sheetId="6" r:id="rId2"/>
+    <x:sheet name="SalesOrderActual" sheetId="7" r:id="rId3"/>
+    <x:sheet name="SalesOrderBalanceSheet" sheetId="8" r:id="rId4"/>
+    <x:sheet name="CustomerSheet" sheetId="9" r:id="rId5"/>
   </x:sheets>
   <x:definedNames>
     <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",#REF!,#REF!,"none")</x:definedName>
@@ -65,30 +64,8 @@
 </x:workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="91">
   <si>
     <t>StartDate</t>
   </si>
@@ -361,12 +338,6 @@
   </si>
   <si>
     <t>ShippingAgentCode</t>
-  </si>
-  <si>
-    <t>Document Type</t>
-  </si>
-  <si>
-    <t>Document No.</t>
   </si>
 </sst>
 </file>
@@ -556,7 +527,7 @@
     <x:tableColumn id="1" name="StartDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="2" name="EndDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -596,7 +567,7 @@
     <x:tableColumn id="30" name="Calculated" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="31" name="CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -629,7 +600,7 @@
     <x:tableColumn id="23" name="CustomerGroupCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="24" name="CustomerPostingGroup111" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -662,7 +633,7 @@
     <x:tableColumn id="23" name="CustomerGroupCode222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="24" name="CustomerPostingGroup222" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -679,7 +650,7 @@
     <x:tableColumn id="7" name="ShipmentMethodCode333" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="8" name="ShippingAgentCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -982,13 +953,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33CD324A-2965-41B1-8AFF-2478309124C6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1020,7 +992,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1227,133 +1199,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{805EF4CF-BE6F-49F8-8F1B-CC10C3643A3F}">
-  <dimension ref="A1:AE2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>91</v>
-      </c>
-      <c r="B1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:AE2">RemainingSalesOrder[]</f>
-        <v/>
-      </c>
-      <c r="B2" t="str">
-        <v/>
-      </c>
-      <c r="C2" t="str">
-        <v/>
-      </c>
-      <c r="D2" t="str">
-        <v/>
-      </c>
-      <c r="E2" t="str">
-        <v/>
-      </c>
-      <c r="F2" t="str">
-        <v/>
-      </c>
-      <c r="G2" t="str">
-        <v/>
-      </c>
-      <c r="H2" t="str">
-        <v/>
-      </c>
-      <c r="I2" t="str">
-        <v/>
-      </c>
-      <c r="J2" t="str">
-        <v/>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="str">
-        <v/>
-      </c>
-      <c r="O2" t="str">
-        <v/>
-      </c>
-      <c r="P2" t="str">
-        <v/>
-      </c>
-      <c r="Q2" t="str">
-        <v/>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2" t="str">
-        <v>False</v>
-      </c>
-      <c r="U2" t="str">
-        <v/>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2" t="str">
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF22EC56-EE68-4288-9303-7A32AEBCCC8E}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1517,7 +1367,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AC93CF-A70D-4E86-AA46-4AE1A32EDE8E}">
   <dimension ref="A1:X2"/>
   <sheetViews>
@@ -1684,12 +1534,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCE851F-52AC-4D40-872D-5DA20E49CF56}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Report(Actual Order Amount & Order Balance) updated: the layout of excel
</commit_message>
<xml_diff>
--- a/XLSX/ActualOrderAmountOrderBalance.xlsx
+++ b/XLSX/ActualOrderAmountOrderBalance.xlsx
@@ -1,62 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
-  <x:workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\Hagiwara\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92869846-AC51-487B-8BAE-6BE901ADBEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="903" firstSheet="7" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </x:bookViews>
-  <x:sheets>
-    <x:sheet name="TranslationData" sheetId="2" state="hidden" r:id="rId1"/>
-    <x:sheet name="CaptionData" sheetId="3" state="hidden" r:id="rId2"/>
-    <x:sheet name="Aggregated Metadata" sheetId="4" state="hidden" r:id="rId3"/>
-    <x:sheet name="RemainingSalesOrder" sheetId="6" state="hidden" r:id="rId4"/>
-    <x:sheet name="SalesOrderActual" sheetId="7" state="hidden" r:id="rId5"/>
-    <x:sheet name="SalesOrderBalance" sheetId="8" state="hidden" r:id="rId6"/>
-    <x:sheet name="CustomerSheet" sheetId="9" state="hidden" r:id="rId7"/>
-    <x:sheet name="Date" sheetId="5" r:id="rId8"/>
-    <x:sheet name="Remaining Sales Order" sheetId="10" r:id="rId9"/>
-    <x:sheet name="Sales Order Actual" sheetId="11" r:id="rId10"/>
-    <x:sheet name="Sales Order Balance" sheetId="12" r:id="rId11"/>
-    <x:sheet name="Customer" sheetId="13" r:id="rId12"/>
-  </x:sheets>
-  <x:definedNames>
-    <x:definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension Id from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ObjectCaption" comment="Use this function to get the Object Caption from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Caption",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company Display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.DateLocal" comment="Use this function to get the Date (Local) from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date (Local)",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-    <x:definedName name="ReportRequest.UTCOffset" comment="Use this function to get the UTC Offset from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("UTC Offset",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</x:definedName>
-  </x:definedNames>
-  <x:calcPr calcId="191029"/>
-  <x:extLst>
-    <x:ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129F1370-FBB0-4F65-9A43-C64E1FBF98B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" firstSheet="8" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="TranslationData" sheetId="2" state="hidden" r:id="rId1"/>
+    <sheet name="CaptionData" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Aggregated Metadata" sheetId="4" state="hidden" r:id="rId3"/>
+    <sheet name="DateSheet" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="RemainingSalesOrder" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="SalesOrderActual" sheetId="7" state="hidden" r:id="rId6"/>
+    <sheet name="SalesOrderBalance" sheetId="8" state="hidden" r:id="rId7"/>
+    <sheet name="CustomerSheet" sheetId="9" state="hidden" r:id="rId8"/>
+    <sheet name="Date" sheetId="14" r:id="rId9"/>
+    <sheet name="Remaining Sales Order" sheetId="10" r:id="rId10"/>
+    <sheet name="Sales Order Actual" sheetId="11" r:id="rId11"/>
+    <sheet name="Sales Order Balance" sheetId="12" r:id="rId12"/>
+    <sheet name="Customer" sheetId="13" r:id="rId13"/>
+  </sheets>
+  <definedNames>
+    <definedName name="ReportMetadata.AboutThisReportText" comment="Use this function to get the About This Report Text from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Text",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.AboutThisReportTitle" comment="Use this function to get the About This Report Title from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("About This Report Title",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionID" comment="Use this function to get the Extension Id from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionName" comment="Use this function to get the Extension Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionPublisher" comment="Use this function to get the Extension Publisher from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Publisher",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ExtensionVersion" comment="Use this function to get the Extension Version from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Extension Version",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ObjectCaption" comment="Use this function to get the Object Caption from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Caption",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ObjectID" comment="Use this function to get the Object ID from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object ID",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ObjectName" comment="Use this function to get the Object Name from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Object Name",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportMetadata.ReportHelpLink" comment="Use this function to get the Report help link from the ReportMetadataValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Report help link",ReportMetadataValues[[#All],[Report Property]],ReportMetadataValues[[#All],[Report Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.CompanyDisplayName" comment="Use this function to get the Company Display name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company display name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.CompanyId" comment="Use this function to get the Company Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.CompanyName" comment="Use this function to get the Company name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Company name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.Date" comment="Use this function to get the Date from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.DateLocal" comment="Use this function to get the Date (Local) from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Date (Local)",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.EnvironmentName" comment="Use this function to get the Environment name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.EnvironmentType" comment="Use this function to get the Environment type from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Environment type",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.FormatRegion" comment="Use this function to get the Format Region from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Format Region",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.Language" comment="Use this function to get the Language from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Language",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.LayoutCaption" comment="Use this function to get the Layout caption from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout caption",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.LayoutId" comment="Use this function to get the Layout id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.LayoutName" comment="Use this function to get the Layout name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Layout name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.TenantEntraId" comment="Use this function to get the Tenant Entra Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Entra Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.TenantId" comment="Use this function to get the Tenant Id from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("Tenant Id",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.UserName" comment="Use this function to get the User name from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("User name",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+    <definedName name="ReportRequest.UTCOffset" comment="Use this function to get the UTC Offset from the ReportRequestValues table in the Aggregated Metadata worksheet">_xlfn.XLOOKUP("UTC Offset",ReportRequestValues[[#All],[Request Property]],ReportRequestValues[[#All],[Request Property Value]],"none")</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
@@ -66,9 +67,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
-    </x:ext>
-  </x:extLst>
-</x:workbook>
+    </ext>
+  </extLst>
+</workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="210">
   <si>
     <t>Language</t>
   </si>
@@ -1033,31 +1034,53 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:H2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="8">
-    <x:tableColumn id="1" name="CU_No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="CU_FamiliarName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="3" name="CU_Name" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="4" name="CU_CountryRegionCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="5" name="CU_County" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="6" name="CU_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="7" name="CU_ShipmentMethodCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="8" name="CU_ShippingAgentCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="SalesOrderBalance" displayName="SalesOrderBalance" ref="A1:X2" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_ShipmentDate"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_PostingDate"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_DocumentDate"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_No"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_CustomerNo"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_Customer"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_OrderNo"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_OEMNo"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_OEMName"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_CurrencyCode"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_DueDate"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_Amount"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_AmountLCY"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_AmountIncludingVAT"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_ExternalDocumentNo"/>
+    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_RemainingAmount"/>
+    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_LocationCode"/>
+    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_PrintedNo"/>
+    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_Closed"/>
+    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_Cancelled"/>
+    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_Corrective"/>
+    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_ShipmentMethodCode"/>
+    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_CustomerGroupCode"/>
+    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="BAL_CustomerPostingGroup"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Date" displayName="Date" ref="A1:B2" totalsRowShown="0" headerRowDxfId="4" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:B2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="2">
-    <x:tableColumn id="1" name="From" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="To" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:H2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_No"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_FamiliarName"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_Name"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_CountryRegionCode"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_County"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_CustomerPostingGroup"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_ShipmentMethodCode"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="CU_ShippingAgentCode"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1116,109 +1139,87 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="3" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="31">
-    <x:tableColumn id="1" name="SO_DocumentType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="SO_DocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="3" name="SO_SelltoCustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="4" name="SO_Type" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="5" name="SO_No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="6" name="SO_CustomerItemNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="7" name="SO_PartsNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="8" name="SO_Rank" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="9" name="SO_Products" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="10" name="SO_OEMNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="11" name="SO_OrderDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="12" name="SO_PromisedDeliveryDate1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="13" name="SO_RequestedDeliveryDate1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="14" name="SO_Description" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="15" name="SO_CustomerOrderNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="16" name="SO_LocationCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="17" name="SO_Reserve" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="18" name="SO_Quantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="19" name="SO_ReservedQtyBase" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="20" name="SO_FullyReserved" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="21" name="SO_UnitofMeasureCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="22" name="SO_UnitPriceExcl_VAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="23" name="SO_UnitCost" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="24" name="SO_UnitCost_LCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="25" name="SO_LineAmountExclVAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="26" name="SO_LineAmountExclVATLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="27" name="SO_ShipmentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="28" name="SO_OutstandingQuantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="29" name="SO_OutstandingQtyBase" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="30" name="SO_Calculated" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="31" name="SO_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="DateSheet" displayName="DateSheet" ref="A1:B2" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A1:B2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="From"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="To"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="24">
-    <x:tableColumn id="1" name="ACT_ShipmentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="ACT_PostingDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="3" name="ACT_DocumentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="4" name="ACT_No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="5" name="ACT_CustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="6" name="ACT_Customer" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="7" name="ACT_OrderNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="8" name="ACT_OEMNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="9" name="ACT_OEMName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="10" name="ACT_CurrencyCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="11" name="ACT_DueDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="12" name="ACT_Amount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="13" name="ACT_AmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="14" name="ACT_AmountIncludingVAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="15" name="ACT_ExternalDocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="16" name="ACT_RemainingAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="17" name="ACT_LocationCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="18" name="ACT_PrintedNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="19" name="ACT_Closed" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="20" name="ACT_Cancelled" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="21" name="ACT_Corrective" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="22" name="ACT_ShipmentMethodCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="23" name="ACT_CustomerGroupCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="24" name="ACT_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="31">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_DocumentType"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_DocumentNo"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_SelltoCustomerNo"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Type"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_No"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_CustomerItemNo"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_PartsNo"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Rank"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Products"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_OEMNo"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_OrderDate"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_PromisedDeliveryDate1"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_RequestedDeliveryDate1"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Description"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_CustomerOrderNo"/>
+    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_LocationCode"/>
+    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Reserve"/>
+    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Quantity"/>
+    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_ReservedQtyBase"/>
+    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_FullyReserved"/>
+    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_UnitofMeasureCode"/>
+    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_UnitPriceExcl_VAT"/>
+    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_UnitCost"/>
+    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_UnitCost_LCY"/>
+    <tableColumn id="25" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_LineAmountExclVAT"/>
+    <tableColumn id="26" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_LineAmountExclVATLCY"/>
+    <tableColumn id="27" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_ShipmentDate"/>
+    <tableColumn id="28" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_OutstandingQuantity"/>
+    <tableColumn id="29" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_OutstandingQtyBase"/>
+    <tableColumn id="30" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_Calculated"/>
+    <tableColumn id="31" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SO_CustomerPostingGroup"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SalesOrderBalance" displayName="SalesOrderBalance" ref="A1:X2" totalsRowShown="0" headerRowDxfId="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="24">
-    <x:tableColumn id="1" name="BAL_ShipmentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="2" name="BAL_PostingDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="3" name="BAL_DocumentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="4" name="BAL_No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="5" name="BAL_CustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="6" name="BAL_Customer" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="7" name="BAL_OrderNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="8" name="BAL_OEMNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="9" name="BAL_OEMName" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="10" name="BAL_CurrencyCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="11" name="BAL_DueDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="12" name="BAL_Amount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="13" name="BAL_AmountLCY" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="14" name="BAL_AmountIncludingVAT" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="15" name="BAL_ExternalDocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="16" name="BAL_RemainingAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="17" name="BAL_LocationCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="18" name="BAL_PrintedNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="19" name="BAL_Closed" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="20" name="BAL_Cancelled" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="21" name="BAL_Corrective" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="22" name="BAL_ShipmentMethodCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="23" name="BAL_CustomerGroupCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-    <x:tableColumn id="24" name="BAL_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
-  </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</x:table>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_ShipmentDate"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_PostingDate"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_DocumentDate"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_No"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_CustomerNo"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_Customer"/>
+    <tableColumn id="7" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_OrderNo"/>
+    <tableColumn id="8" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_OEMNo"/>
+    <tableColumn id="9" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_OEMName"/>
+    <tableColumn id="10" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_CurrencyCode"/>
+    <tableColumn id="11" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_DueDate"/>
+    <tableColumn id="12" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_Amount"/>
+    <tableColumn id="13" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_AmountLCY"/>
+    <tableColumn id="14" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_AmountIncludingVAT"/>
+    <tableColumn id="15" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_ExternalDocumentNo"/>
+    <tableColumn id="16" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_RemainingAmount"/>
+    <tableColumn id="17" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_LocationCode"/>
+    <tableColumn id="18" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_PrintedNo"/>
+    <tableColumn id="19" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_Closed"/>
+    <tableColumn id="20" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_Cancelled"/>
+    <tableColumn id="21" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_Corrective"/>
+    <tableColumn id="22" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_ShipmentMethodCode"/>
+    <tableColumn id="23" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_CustomerGroupCode"/>
+    <tableColumn id="24" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ACT_CustomerPostingGroup"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1517,11 +1518,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13D73E4-6957-4462-8115-AB0B1AC0F9C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE03138-0977-4CE7-8942-BE841E10F132}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1550,11 +1551,217 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC1680F9-1A30-478C-BD94-7D1850267C70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB76EA3-A1F9-4902-A3A6-D1EF60E803D5}">
+  <dimension ref="A1:AE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" t="s">
+        <v>161</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N1" t="s">
+        <v>168</v>
+      </c>
+      <c r="O1" t="s">
+        <v>169</v>
+      </c>
+      <c r="P1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>171</v>
+      </c>
+      <c r="R1" t="s">
+        <v>172</v>
+      </c>
+      <c r="S1" t="s">
+        <v>173</v>
+      </c>
+      <c r="T1" t="s">
+        <v>174</v>
+      </c>
+      <c r="U1" t="s">
+        <v>175</v>
+      </c>
+      <c r="V1" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" t="s">
+        <v>177</v>
+      </c>
+      <c r="X1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>180</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>182</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>183</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="A2" t="str" cm="1">
+        <f t="array" ref="A2:AE2">RemainingSalesOrder[]</f>
+        <v/>
+      </c>
+      <c r="B2" t="str">
+        <v/>
+      </c>
+      <c r="C2" t="str">
+        <v/>
+      </c>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="str">
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <v/>
+      </c>
+      <c r="P2" t="str">
+        <v/>
+      </c>
+      <c r="Q2" t="str">
+        <v/>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2" t="str">
+        <v>False</v>
+      </c>
+      <c r="U2" t="str">
+        <v/>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="str">
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465EB37D-E0F3-49FC-804F-5BFB5B1A97C4}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1713,12 +1920,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06034408-6E5C-459E-8FF2-0E8EFA52399E}">
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB99276-2F13-477C-8C83-7DBBF28DE91B}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1808,26 +2015,26 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="D2" t="str">
+        <v/>
+      </c>
+      <c r="E2" t="str">
+        <v/>
+      </c>
+      <c r="F2" t="str">
+        <v/>
+      </c>
+      <c r="G2" t="str">
+        <v/>
+      </c>
+      <c r="H2" t="str">
+        <v/>
+      </c>
+      <c r="I2" t="str">
+        <v/>
+      </c>
+      <c r="J2" t="str">
+        <v/>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1841,35 +2048,35 @@
       <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2">
-        <v>0</v>
+      <c r="O2" t="str">
+        <v/>
       </c>
       <c r="P2">
         <v>0</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
+      <c r="Q2" t="str">
+        <v/>
       </c>
       <c r="R2">
         <v>0</v>
       </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
+      <c r="S2" t="str">
+        <v>False</v>
+      </c>
+      <c r="T2" t="str">
+        <v>False</v>
+      </c>
+      <c r="U2" t="str">
+        <v>False</v>
+      </c>
+      <c r="V2" t="str">
+        <v/>
+      </c>
+      <c r="W2" t="str">
+        <v/>
+      </c>
+      <c r="X2" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
@@ -1877,12 +2084,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB1B0179-4D69-4EA7-AD1E-4707826746C8}">
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93257168-34BE-4386-8A8A-E38C5A76A296}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1946,11 +2153,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A584DBC8-F669-4099-99CA-87A3026B2893}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A19B756-E7EA-4713-8A8E-022F402BFCB7}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1984,11 +2191,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C7F984-ECF7-4495-B1E0-1CA94C534DF1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F20EBC-EE4B-46D0-8CE3-C210A0569D8A}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2244,11 +2451,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E97FCF8-1173-40C6-A501-80EDBD1AE557}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA82CC89-6D06-4756-8B0B-4A54FCE7A423}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06151AC8-45FC-411C-A803-522D383BFE68}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2352,20 +2596,99 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="2"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>97</v>
+      </c>
+      <c r="O2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" t="s">
+        <v>97</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2375,12 +2698,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D9E0BE3-A94A-4DCB-9F52-9E941825EC13}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E46625-F99B-4A95-996C-7A0A90370764}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2544,12 +2867,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3156EC8D-C25C-44C3-9720-DB9C271E4B9D}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A38B6F-A117-4B92-B162-BC9B3E61C0B1}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2632,15 +2955,78 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="R2" s="4"/>
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
+      </c>
+      <c r="G2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H2" t="s">
+        <v>97</v>
+      </c>
+      <c r="I2" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>97</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>98</v>
+      </c>
+      <c r="T2" t="s">
+        <v>98</v>
+      </c>
+      <c r="U2" t="s">
+        <v>98</v>
+      </c>
+      <c r="V2" t="s">
+        <v>97</v>
+      </c>
+      <c r="W2" t="s">
+        <v>97</v>
+      </c>
+      <c r="X2" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2650,12 +3036,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B1848C-B48C-4BEE-8114-7ED3FFF26016}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7EDFF4-0711-417B-A3E5-FF79C127E457}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2723,18 +3109,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC15C187-ED39-4EFA-BA83-55EB60662E18}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C53E28-5C5C-488C-8B9C-E27EF8250F65}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -2745,215 +3126,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AB1899-C31A-434F-84D3-3FD8D0B93414}">
-  <dimension ref="A1:AE2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" t="s">
-        <v>158</v>
-      </c>
-      <c r="E1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" t="s">
-        <v>160</v>
-      </c>
-      <c r="G1" t="s">
-        <v>161</v>
-      </c>
-      <c r="H1" t="s">
-        <v>162</v>
-      </c>
-      <c r="I1" t="s">
-        <v>163</v>
-      </c>
-      <c r="J1" t="s">
-        <v>164</v>
-      </c>
-      <c r="K1" t="s">
-        <v>165</v>
-      </c>
-      <c r="L1" t="s">
-        <v>166</v>
-      </c>
-      <c r="M1" t="s">
-        <v>167</v>
-      </c>
-      <c r="N1" t="s">
-        <v>168</v>
-      </c>
-      <c r="O1" t="s">
-        <v>169</v>
-      </c>
-      <c r="P1" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>171</v>
-      </c>
-      <c r="R1" t="s">
-        <v>172</v>
-      </c>
-      <c r="S1" t="s">
-        <v>173</v>
-      </c>
-      <c r="T1" t="s">
-        <v>174</v>
-      </c>
-      <c r="U1" t="s">
-        <v>175</v>
-      </c>
-      <c r="V1" t="s">
-        <v>176</v>
-      </c>
-      <c r="W1" t="s">
-        <v>177</v>
-      </c>
-      <c r="X1" t="s">
-        <v>178</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>179</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>180</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>181</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>182</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>183</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A2" cm="1">
-        <f t="array" ref="A2:AE2">RemainingSalesOrder[]</f>
+        <f t="array" ref="A2:B2">DateSheet[]</f>
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
-      </c>
-      <c r="Y2">
-        <v>0</v>
-      </c>
-      <c r="Z2">
-        <v>0</v>
-      </c>
-      <c r="AA2">
-        <v>0</v>
-      </c>
-      <c r="AB2">
-        <v>0</v>
-      </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
-        <v>0</v>
-      </c>
-      <c r="AE2">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Report(Actual Order Amount & Order Balance) updated: the Tooltip and Validation for from and to etc.
</commit_message>
<xml_diff>
--- a/XLSX/ActualOrderAmountOrderBalance.xlsx
+++ b/XLSX/ActualOrderAmountOrderBalance.xlsx
@@ -5,12 +5,12 @@
   <x:workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\Hagiwara\XLSX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E116DC-0184-4E69-A5AC-A14224F13417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35E305B-84C3-4192-9471-C41940039FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Date" sheetId="14" r:id="rId1"/>
@@ -731,6 +731,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -790,20 +793,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -815,20 +819,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1097,7 +1087,7 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SalesOrderBalance" displayName="SalesOrderBalance" ref="A1:X2" totalsRowShown="0" headerRowDxfId="7" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="SalesOrderBalance" displayName="SalesOrderBalance" ref="A1:X2" totalsRowShown="0" headerRowDxfId="5" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
   <x:autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
   <x:tableColumns count="24">
     <x:tableColumn id="1" name="BAL_ShipmentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
@@ -1130,7 +1120,7 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="6" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="CustomerSheet" displayName="CustomerSheet" ref="A1:H2" totalsRowShown="0" headerRowDxfId="4" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
   <x:autoFilter ref="A1:H2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
   <x:tableColumns count="8">
     <x:tableColumn id="1" name="CU_No" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
@@ -1158,7 +1148,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{134EB915-8B19-4838-BDED-CECBACACF4F9}" name="ReportMetadataValues" displayName="ReportMetadataValues" ref="A1:B11" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{134EB915-8B19-4838-BDED-CECBACACF4F9}" name="ReportMetadataValues" displayName="ReportMetadataValues" ref="A1:B11" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:B11" xr:uid="{134EB915-8B19-4838-BDED-CECBACACF4F9}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5CBC1C08-5A8D-42BB-92CA-C3F1D0EF0A4D}" name="Report Property"/>
@@ -1169,7 +1159,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1DFF5EE2-2A86-40DE-9DFD-1E96553323F6}" name="ReportRequestValues" displayName="ReportRequestValues" ref="D1:E17" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1DFF5EE2-2A86-40DE-9DFD-1E96553323F6}" name="ReportRequestValues" displayName="ReportRequestValues" ref="D1:E17" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="D1:E17" xr:uid="{1DFF5EE2-2A86-40DE-9DFD-1E96553323F6}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{E6EF2D44-8AB2-42E8-A7E3-9B148922AA59}" name="Request Property"/>
@@ -1180,7 +1170,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8D3A40BA-47FA-41F3-82A4-C5BD4909C0B4}" name="ReportRequestPageValues" displayName="ReportRequestPageValues" ref="G1:H2" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8D3A40BA-47FA-41F3-82A4-C5BD4909C0B4}" name="ReportRequestPageValues" displayName="ReportRequestPageValues" ref="G1:H2" totalsRowShown="0" headerRowDxfId="10">
   <autoFilter ref="G1:H2" xr:uid="{8D3A40BA-47FA-41F3-82A4-C5BD4909C0B4}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{023648B2-C225-4580-B767-C48467418032}" name="Request Page Option"/>
@@ -1191,7 +1181,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D269260C-C433-478B-84A3-3CB73C333872}" name="ReportFilterValues" displayName="ReportFilterValues" ref="J1:K2" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D269260C-C433-478B-84A3-3CB73C333872}" name="ReportFilterValues" displayName="ReportFilterValues" ref="J1:K2" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="J1:K2" xr:uid="{D269260C-C433-478B-84A3-3CB73C333872}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D710F0AA-F8F4-4DB2-BC43-E65C2054A321}" name="Filter"/>
@@ -1202,7 +1192,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="DateSheet" displayName="DateSheet" ref="A1:B2" totalsRowShown="0" headerRowDxfId="10" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="DateSheet" displayName="DateSheet" ref="A1:B2" totalsRowShown="0" headerRowDxfId="8" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
   <x:autoFilter ref="A1:B2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
   <x:tableColumns count="2">
     <x:tableColumn id="1" name="From" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
@@ -1213,7 +1203,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="9" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="7" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
   <x:autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
   <x:tableColumns count="31">
     <x:tableColumn id="1" name="SO_DocumentType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
@@ -1253,7 +1243,7 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="8" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="SalesOrderActual" displayName="SalesOrderActual" ref="A1:X2" totalsRowShown="0" headerRowDxfId="6" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
   <x:autoFilter ref="A1:X2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
   <x:tableColumns count="24">
     <x:tableColumn id="1" name="ACT_ShipmentDate" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
@@ -1584,7 +1574,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C53E28-5C5C-488C-8B9C-E27EF8250F65}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1600,11 +1592,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+      <c r="A2" s="7">
         <f>DateSheet[[#This Row],[From]]</f>
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="7">
         <f>DateSheet[[#This Row],[To]]</f>
         <v>0</v>
       </c>
@@ -1619,12 +1611,13 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
@@ -2240,107 +2233,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB76EA3-A1F9-4902-A3A6-D1EF60E803D5}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1796875" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.90625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.81640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="21.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Y1" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AB1" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="6" t="s">
         <v>185</v>
       </c>
     </row>
@@ -2376,13 +2398,13 @@
       <c r="J2" t="str">
         <v/>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
+      <c r="K2" s="8">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8">
         <v>0</v>
       </c>
       <c r="N2" t="str">
@@ -2424,7 +2446,7 @@
       <c r="Z2">
         <v>0</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="8">
         <v>0</v>
       </c>
       <c r="AB2">
@@ -2442,7 +2464,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2455,14 +2477,14 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
@@ -2470,6 +2492,7 @@
     <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
@@ -2486,88 +2509,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" cm="1">
+      <c r="A2" s="8" cm="1">
         <f t="array" ref="A2:X2">SalesOrderActual[]</f>
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
         <v>0</v>
       </c>
       <c r="D2" t="str">
@@ -2591,7 +2614,7 @@
       <c r="J2" t="str">
         <v/>
       </c>
-      <c r="K2">
+      <c r="K2" s="8">
         <v>0</v>
       </c>
       <c r="L2">
@@ -2636,7 +2659,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2648,15 +2671,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB99276-2F13-477C-8C83-7DBBF28DE91B}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.90625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
@@ -2664,7 +2687,7 @@
     <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.453125" style="8" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
@@ -2681,88 +2704,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="Q1" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="U1" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="V1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="W1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="6" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" cm="1">
+      <c r="A2" s="8" cm="1">
         <f t="array" ref="A2:X2">SalesOrderBalance[]</f>
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
+      <c r="B2" s="8">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8">
         <v>0</v>
       </c>
       <c r="D2" t="str">
@@ -2786,7 +2809,7 @@
       <c r="J2" t="str">
         <v/>
       </c>
-      <c r="K2">
+      <c r="K2" s="8">
         <v>0</v>
       </c>
       <c r="L2">
@@ -2831,7 +2854,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:XFD1048576">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2843,8 +2866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93257168-34BE-4386-8A8A-E38C5A76A296}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2860,28 +2883,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>209</v>
       </c>
     </row>

</xml_diff>

<commit_message>
N005 Availality based on Approved Quantity.
</commit_message>
<xml_diff>
--- a/XLSX/ActualOrderAmountOrderBalance.xlsx
+++ b/XLSX/ActualOrderAmountOrderBalance.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <x:workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Hagiwara-Upgrade\AL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ShawnLi\Documents\Cals\Hagiwara_Upgrade\BC\AL\Hagiwara\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35E305B-84C3-4192-9471-C41940039FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C4CB2E-9AF3-443E-AACB-A6186488D02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="859" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet name="Date" sheetId="14" r:id="rId1"/>
-    <x:sheet name="Remaining Sales Order" sheetId="10" r:id="rId2"/>
-    <x:sheet name="Sales Order Actual" sheetId="11" r:id="rId3"/>
-    <x:sheet name="Sales Order Balance" sheetId="12" r:id="rId4"/>
-    <x:sheet name="Customer" sheetId="13" r:id="rId5"/>
+    <x:sheet name="Date" sheetId="10" r:id="rId1"/>
+    <x:sheet name="Remaining Sales Order" sheetId="11" r:id="rId2"/>
+    <x:sheet name="Sales Order Actual" sheetId="12" r:id="rId3"/>
+    <x:sheet name="Sales Order Balance" sheetId="13" r:id="rId4"/>
+    <x:sheet name="Customer" sheetId="14" r:id="rId5"/>
     <x:sheet name="TranslationData" sheetId="2" state="hidden" r:id="rId6"/>
     <x:sheet name="CaptionData" sheetId="3" state="hidden" r:id="rId7"/>
     <x:sheet name="Aggregated Metadata" sheetId="4" state="hidden" r:id="rId8"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="216">
   <si>
     <t>Language</t>
   </si>
@@ -388,6 +388,15 @@
     <t>SO_CustomerPostingGroup</t>
   </si>
   <si>
+    <t>SO_ApprovedQuantity</t>
+  </si>
+  <si>
+    <t>SO_ApprovedUnitPrice</t>
+  </si>
+  <si>
+    <t>SO_ApprovedAmount</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
@@ -725,6 +734,18 @@
   </si>
   <si>
     <t>Shipping Agent Code</t>
+  </si>
+  <si>
+    <t>Approved Quantity</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Approved Unit Price</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Approved Amount Excl. VAT</t>
+    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -732,20 +753,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="176" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -800,12 +828,12 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
     <dxf>
@@ -1115,7 +1143,7 @@
     <x:tableColumn id="23" name="BAL_CustomerGroupCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="24" name="BAL_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -1132,7 +1160,7 @@
     <x:tableColumn id="7" name="CU_ShipmentMethodCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="8" name="CU_ShippingAgentCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -1198,14 +1226,14 @@
     <x:tableColumn id="1" name="From" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="2" name="To" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AE2" totalsRowShown="0" headerRowDxfId="7" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
-  <x:autoFilter ref="A1:AE2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <x:tableColumns count="31">
+<x:table xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="RemainingSalesOrder" displayName="RemainingSalesOrder" ref="A1:AH2" totalsRowShown="0" headerRowDxfId="7" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" mc:Ignorable="xr xr3">
+  <x:autoFilter ref="A1:AH2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <x:tableColumns count="34">
     <x:tableColumn id="1" name="SO_DocumentType" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="2" name="SO_DocumentNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="3" name="SO_SelltoCustomerNo" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
@@ -1237,8 +1265,11 @@
     <x:tableColumn id="29" name="SO_OutstandingQtyBase" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="30" name="SO_Calculated" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="31" name="SO_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="32" name="SO_ApprovedQuantity" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="33" name="SO_ApprovedUnitPrice" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
+    <x:tableColumn id="34" name="SO_ApprovedAmount" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
@@ -1271,12 +1302,12 @@
     <x:tableColumn id="23" name="ACT_CustomerGroupCode" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
     <x:tableColumn id="24" name="ACT_CustomerPostingGroup" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}"/>
   </x:tableColumns>
-  <x:tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <x:tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -1571,19 +1602,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C53E28-5C5C-488C-8B9C-E27EF8250F65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2288BB9B-6709-47CB-B7C9-817F1E183987}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>64</v>
       </c>
@@ -1591,36 +1622,36 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="7">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="6">
         <f>DateSheet[[#This Row],[From]]</f>
         <v>0</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <f>DateSheet[[#This Row],[To]]</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06151AC8-45FC-411C-A803-522D383BFE68}">
-  <dimension ref="A1:AE2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27192392-EA00-44B3-AE44-538F8098BAFA}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>66</v>
       </c>
@@ -1714,37 +1745,46 @@
       <c r="AE1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AF1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
@@ -1756,16 +1796,16 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="P2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="Q2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="R2" s="3">
         <v>0</v>
@@ -1774,10 +1814,10 @@
         <v>0</v>
       </c>
       <c r="T2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="U2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="V2" s="3">
         <v>0</v>
@@ -1807,10 +1847,20 @@
         <v>0</v>
       </c>
       <c r="AE2" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="AF2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1819,167 +1869,168 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E46625-F99B-4A95-996C-7A0A90370764}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92DA9B0-E3EE-41F4-96E1-D3C723C10EF1}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J1" t="s">
+        <v>111</v>
+      </c>
+      <c r="K1" t="s">
+        <v>112</v>
+      </c>
+      <c r="L1" t="s">
+        <v>113</v>
+      </c>
+      <c r="M1" t="s">
+        <v>114</v>
+      </c>
+      <c r="N1" t="s">
+        <v>115</v>
+      </c>
+      <c r="O1" t="s">
+        <v>116</v>
+      </c>
+      <c r="P1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>118</v>
+      </c>
+      <c r="R1" t="s">
+        <v>119</v>
+      </c>
+      <c r="S1" t="s">
+        <v>120</v>
+      </c>
+      <c r="T1" t="s">
+        <v>121</v>
+      </c>
+      <c r="U1" t="s">
+        <v>122</v>
+      </c>
+      <c r="V1" t="s">
+        <v>123</v>
+      </c>
+      <c r="W1" t="s">
+        <v>124</v>
+      </c>
+      <c r="X1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>100</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>100</v>
+      </c>
+      <c r="R2" s="4">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E1" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" t="s">
-        <v>105</v>
-      </c>
-      <c r="H1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" t="s">
-        <v>108</v>
-      </c>
-      <c r="K1" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" t="s">
-        <v>110</v>
-      </c>
-      <c r="M1" t="s">
-        <v>111</v>
-      </c>
-      <c r="N1" t="s">
-        <v>112</v>
-      </c>
-      <c r="O1" t="s">
-        <v>113</v>
-      </c>
-      <c r="P1" t="s">
-        <v>114</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>115</v>
-      </c>
-      <c r="R1" t="s">
-        <v>116</v>
-      </c>
-      <c r="S1" t="s">
-        <v>117</v>
-      </c>
-      <c r="T1" t="s">
-        <v>118</v>
-      </c>
-      <c r="U1" t="s">
-        <v>119</v>
-      </c>
-      <c r="V1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W1" t="s">
-        <v>121</v>
-      </c>
-      <c r="X1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H2" t="s">
-        <v>97</v>
-      </c>
-      <c r="I2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>97</v>
-      </c>
-      <c r="P2" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>97</v>
-      </c>
-      <c r="R2" s="4">
-        <v>0</v>
-      </c>
-      <c r="S2" t="s">
-        <v>98</v>
-      </c>
       <c r="T2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="U2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="V2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="X2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1988,93 +2039,93 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A38B6F-A117-4B92-B162-BC9B3E61C0B1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A66A90A-21D5-44F1-8F52-486D346401A5}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="E1" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="F1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G1" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H1" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="I1" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="J1" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="K1" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="M1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="N1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="O1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="P1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="Q1" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="R1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="S1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="T1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="U1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="V1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="W1" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="X1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -2085,25 +2136,25 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="K2" s="2">
         <v>0</v>
@@ -2118,37 +2169,38 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="P2" s="3">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="R2" s="4">
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="T2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="U2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="V2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="W2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="X2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2157,71 +2209,72 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7EDFF4-0711-417B-A3E5-FF79C127E457}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EE184B-5E4B-4589-AF05-0E22CA869E0C}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C1" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E1" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F1" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H1" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2230,145 +2283,154 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB76EA3-A1F9-4902-A3A6-D1EF60E803D5}">
-  <dimension ref="A1:AE2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A35B9210-B6E3-46CF-81BC-9E9F60A92CA5}">
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.36328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.4140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.4140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.4140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.4140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.9140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="6" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="O1" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="P1" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="R1" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="S1" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="T1" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="U1" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="V1" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="W1" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="X1" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="Y1" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="Z1" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AA1" s="7" t="s">
         <v>184</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AB1" s="7" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AC1" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:AE2">RemainingSalesOrder[]</f>
+        <f t="array" ref="A2:AH2">RemainingSalesOrder[#Data]</f>
         <v/>
       </c>
       <c r="B2" t="str">
@@ -2461,8 +2523,18 @@
       <c r="AE2" t="str">
         <v/>
       </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="A2:XFD1048576">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
@@ -2473,118 +2545,118 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{465EB37D-E0F3-49FC-804F-5BFB5B1A97C4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56840D0B-8804-46AE-B3BE-559BAFBC6888}">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.4140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.4140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.4140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="6" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" cm="1">
-        <f t="array" ref="A2:X2">SalesOrderActual[]</f>
+        <f t="array" ref="A2:X2">SalesOrderActual[#Data]</f>
         <v>0</v>
       </c>
       <c r="B2" s="8">
@@ -2658,6 +2730,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="A2:XFD1048576">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
@@ -2668,118 +2741,118 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB99276-2F13-477C-8C83-7DBBF28DE91B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D4F6D3-DFEC-43BB-800E-1779455D7C29}">
   <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.453125" style="8" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.4140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.75" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.6328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.4140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.4140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>186</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E1" s="6" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="X1" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>197</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="W1" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" cm="1">
-        <f t="array" ref="A2:X2">SalesOrderBalance[]</f>
+        <f t="array" ref="A2:X2">SalesOrderBalance[#Data]</f>
         <v>0</v>
       </c>
       <c r="B2" s="8">
@@ -2853,6 +2926,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="A2:XFD1048576">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
@@ -2863,54 +2937,54 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93257168-34BE-4386-8A8A-E38C5A76A296}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D2E03B7-FCA7-4FF6-BEA9-3EE78EADAC61}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="3.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.9140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H1" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:H2">CustomerSheet[]</f>
+        <f t="array" ref="A2:H2">CustomerSheet[#Data]</f>
         <v/>
       </c>
       <c r="B2" t="str">
@@ -2936,6 +3010,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="A2:XFD1048576">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(MOD(ROW(),2)=0, $A2&lt;&gt;"", A$1&lt;&gt;"")</formula>
@@ -2946,20 +3021,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE03138-0977-4CE7-8942-BE841E10F132}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7C3209-4FB4-46E5-B547-2A4209A8ABCA}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2971,6 +3046,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2979,20 +3055,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A19B756-E7EA-4713-8A8E-022F402BFCB7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{422D5196-3FFF-40B1-8A46-5041F28C8F69}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.4140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3000,7 +3076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3009,6 +3085,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3017,29 +3094,29 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F20EBC-EE4B-46D0-8CE3-C210A0569D8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD85515-4283-40F5-8591-E930E868C6F6}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="25.7265625" customWidth="1"/>
-    <col min="2" max="2" width="40.7265625" customWidth="1"/>
-    <col min="3" max="3" width="5.7265625" customWidth="1"/>
-    <col min="4" max="4" width="25.7265625" customWidth="1"/>
-    <col min="5" max="5" width="40.7265625" customWidth="1"/>
-    <col min="6" max="6" width="5.7265625" customWidth="1"/>
-    <col min="7" max="7" width="25.7265625" customWidth="1"/>
-    <col min="8" max="8" width="40.7265625" customWidth="1"/>
-    <col min="9" max="9" width="5.7265625" customWidth="1"/>
-    <col min="10" max="10" width="40.7265625" customWidth="1"/>
-    <col min="11" max="11" width="25.7265625" customWidth="1"/>
+    <col min="1" max="1" width="25.75" customWidth="1"/>
+    <col min="2" max="2" width="40.75" customWidth="1"/>
+    <col min="3" max="3" width="5.75" customWidth="1"/>
+    <col min="4" max="4" width="25.75" customWidth="1"/>
+    <col min="5" max="5" width="40.75" customWidth="1"/>
+    <col min="6" max="6" width="5.75" customWidth="1"/>
+    <col min="7" max="7" width="25.75" customWidth="1"/>
+    <col min="8" max="8" width="40.75" customWidth="1"/>
+    <col min="9" max="9" width="5.75" customWidth="1"/>
+    <col min="10" max="10" width="40.75" customWidth="1"/>
+    <col min="11" max="11" width="25.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3065,7 +3142,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -3091,7 +3168,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -3105,7 +3182,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -3119,7 +3196,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -3133,7 +3210,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -3147,7 +3224,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -3161,7 +3238,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -3175,7 +3252,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -3189,7 +3266,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -3203,7 +3280,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -3217,7 +3294,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D12" t="s">
         <v>62</v>
       </c>
@@ -3225,7 +3302,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D13" t="s">
         <v>0</v>
       </c>
@@ -3233,7 +3310,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D14" t="s">
         <v>43</v>
       </c>
@@ -3241,7 +3318,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D15" t="s">
         <v>52</v>
       </c>
@@ -3249,7 +3326,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" t="s">
         <v>54</v>
       </c>
@@ -3257,7 +3334,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.55000000000000004">
       <c r="D17" t="s">
         <v>56</v>
       </c>
@@ -3266,6 +3343,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="4">
     <tablePart r:id="rId1"/>
@@ -3277,19 +3355,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA82CC89-6D06-4756-8B0B-4A54FCE7A423}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B6BF9F0-EB50-4DC9-A7EE-E7D02518FDBF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -3297,11 +3375,16 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>